<commit_message>
fixed bug & add logic xor
</commit_message>
<xml_diff>
--- a/inputs/TestData1.xlsx
+++ b/inputs/TestData1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nick\Master Degree\Master Project\Programs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NickWork\tina-transform\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6736481F-7802-43C4-90F7-FC6A2568961A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38BBF04-F473-4A95-B5D7-8B44CEB7B6E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{59CE10C9-A357-44B2-B0C1-D4840FF3072D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{59CE10C9-A357-44B2-B0C1-D4840FF3072D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="TestData5" sheetId="7" r:id="rId8"/>
     <sheet name="TestData6" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="68">
   <si>
     <t>ID</t>
   </si>
@@ -240,24 +240,27 @@
   </si>
   <si>
     <t>XOR1</t>
+  </si>
+  <si>
+    <t>XOR2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -266,7 +269,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -354,13 +357,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>77943</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>91352</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -694,27 +697,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2414180-2D19-4C86-B727-4046CC30FBFE}">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.9140625" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.08203125" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.58203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.08203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="15" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -761,7 +764,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -804,14 +807,8 @@
       <c r="O2" t="s">
         <v>27</v>
       </c>
-      <c r="P2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -824,6 +821,9 @@
       <c r="D3">
         <v>3</v>
       </c>
+      <c r="I3" t="s">
+        <v>67</v>
+      </c>
       <c r="J3" t="s">
         <v>27</v>
       </c>
@@ -842,14 +842,8 @@
       <c r="O3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="P3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -883,14 +877,8 @@
       <c r="O4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="P4" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -925,71 +913,106 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="O6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="O7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="J7" t="s">
-        <v>34</v>
-      </c>
-      <c r="K7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="J8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="N8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="N9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" t="s">
         <v>31</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="L9" t="s">
-        <v>34</v>
-      </c>
-      <c r="M9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="L10" t="s">
+        <v>34</v>
+      </c>
+      <c r="M10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M11" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10" xr:uid="{33790ACD-A3AB-43D7-9383-48039305488A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E11" xr:uid="{33790ACD-A3AB-43D7-9383-48039305488A}">
       <formula1>"and, or"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1002,7 +1025,7 @@
           <x14:formula1>
             <xm:f>Configuration!$A$2:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G10 C2:C13</xm:sqref>
+          <xm:sqref>C2:C14 G2:G11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1018,21 +1041,21 @@
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.9140625" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.08203125" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.58203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.08203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="15" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1079,7 +1102,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1092,7 +1115,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1105,7 +1128,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1118,7 +1141,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1131,7 +1154,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -1144,7 +1167,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -1157,7 +1180,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -1170,7 +1193,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -1183,7 +1206,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1194,7 +1217,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1205,7 +1228,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1246,42 +1269,42 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1">
       <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1">
       <c r="A2" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -1299,13 +1322,13 @@
       <selection activeCell="E2" sqref="E2:J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1361,7 +1384,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1417,7 +1440,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1473,7 +1496,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1529,7 +1552,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1552,7 +1575,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1578,7 +1601,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1601,7 +1624,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1627,7 +1650,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1662,13 +1685,13 @@
       <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1724,7 +1747,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1771,7 +1794,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1818,7 +1841,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1865,7 +1888,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1888,7 +1911,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1905,7 +1928,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1922,7 +1945,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1958,13 +1981,13 @@
       <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2023,7 +2046,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2073,7 +2096,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2123,7 +2146,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2175,7 +2198,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2195,7 +2218,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2215,7 +2238,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -2248,13 +2271,13 @@
       <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2313,7 +2336,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2363,7 +2386,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2413,7 +2436,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2464,7 +2487,7 @@
       </c>
       <c r="V4" s="1"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2502,7 +2525,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2527,7 +2550,7 @@
       </c>
       <c r="U6" s="5"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -2571,7 +2594,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22">
       <c r="P10" t="s">
         <v>35</v>
       </c>
@@ -2589,14 +2612,14 @@
       <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="25" width="3.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="25" width="3.85546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2664,7 +2687,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2723,7 +2746,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2782,7 +2805,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2842,7 +2865,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -2902,7 +2925,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -2934,12 +2957,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -3012,17 +3035,17 @@
       <selection activeCell="AK17" sqref="AK17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="18" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="25" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="34" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="41" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="18" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="25" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="34" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="41" width="4.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3138,7 +3161,7 @@
         <v>2.16</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:41">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3245,7 +3268,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:41">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3352,7 +3375,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -3459,7 +3482,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:41">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -3566,7 +3589,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:41">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -3622,7 +3645,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:41">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -3678,7 +3701,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:41">
       <c r="A8" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
fixed bug & add arcline xor group
</commit_message>
<xml_diff>
--- a/inputs/TestData1.xlsx
+++ b/inputs/TestData1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NickWork\tina-transform\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38BBF04-F473-4A95-B5D7-8B44CEB7B6E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78060F9-7226-4A86-85C2-3F8EE2826F7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{59CE10C9-A357-44B2-B0C1-D4840FF3072D}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="68">
   <si>
     <t>ID</t>
   </si>
@@ -700,7 +700,7 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -789,6 +789,9 @@
       <c r="H2">
         <v>50000</v>
       </c>
+      <c r="I2" t="s">
+        <v>67</v>
+      </c>
       <c r="J2" t="s">
         <v>26</v>
       </c>
@@ -840,7 +843,7 @@
         <v>26</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -875,7 +878,7 @@
         <v>27</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:15">

</xml_diff>

<commit_message>
fixed bug & exclude D- DT object
</commit_message>
<xml_diff>
--- a/inputs/TestData1.xlsx
+++ b/inputs/TestData1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NickWork\tina-transform\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78060F9-7226-4A86-85C2-3F8EE2826F7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382A97C0-1F75-49AE-856E-7A1D6A4CC2A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{59CE10C9-A357-44B2-B0C1-D4840FF3072D}"/>
   </bookViews>
@@ -700,7 +700,7 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -819,7 +819,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -840,7 +840,7 @@
         <v>26</v>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>27</v>
@@ -910,7 +910,7 @@
         <v>27</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>27</v>
@@ -945,7 +945,7 @@
         <v>27</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
fixed bug & add new feature & change label
</commit_message>
<xml_diff>
--- a/inputs/TestData1.xlsx
+++ b/inputs/TestData1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NickWork\tina-transform\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382A97C0-1F75-49AE-856E-7A1D6A4CC2A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E70ED8-4D19-432A-B38F-11696E6B5419}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{59CE10C9-A357-44B2-B0C1-D4840FF3072D}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="66">
   <si>
     <t>ID</t>
   </si>
@@ -237,12 +237,6 @@
   </si>
   <si>
     <t>Female</t>
-  </si>
-  <si>
-    <t>XOR1</t>
-  </si>
-  <si>
-    <t>XOR2</t>
   </si>
 </sst>
 </file>
@@ -362,7 +356,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>77943</xdr:colOff>
+      <xdr:colOff>211293</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>91352</xdr:rowOff>
     </xdr:to>
@@ -697,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2414180-2D19-4C86-B727-4046CC30FBFE}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -713,11 +707,10 @@
     <col min="6" max="6" width="17.140625" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="15" width="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="14" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:14">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -742,29 +735,26 @@
       <c r="H1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="7" t="s">
-        <v>63</v>
+      <c r="I1" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -790,7 +780,7 @@
         <v>50000</v>
       </c>
       <c r="I2" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
         <v>26</v>
@@ -802,21 +792,18 @@
         <v>26</v>
       </c>
       <c r="M2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N2" t="s">
         <v>27</v>
       </c>
-      <c r="O2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>54</v>
@@ -825,28 +812,25 @@
         <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="J3" t="s">
         <v>27</v>
       </c>
       <c r="K3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L3" t="s">
         <v>26</v>
       </c>
       <c r="M3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+        <v>27</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -860,28 +844,25 @@
         <v>13</v>
       </c>
       <c r="I4" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="J4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K4" t="s">
         <v>27</v>
       </c>
       <c r="L4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" t="s">
-        <v>26</v>
+        <v>26</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -895,28 +876,25 @@
         <v>65</v>
       </c>
       <c r="I5" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="J5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K5" t="s">
         <v>26</v>
       </c>
       <c r="L5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -930,85 +908,82 @@
         <v>65</v>
       </c>
       <c r="I6" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="J6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K6" t="s">
         <v>26</v>
       </c>
       <c r="L6" t="s">
-        <v>26</v>
-      </c>
-      <c r="M6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="O7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="N7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>16</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
+      <c r="I8" t="s">
+        <v>34</v>
+      </c>
       <c r="J8" t="s">
         <v>34</v>
       </c>
-      <c r="K8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="N9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="M9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>31</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
       </c>
+      <c r="K10" t="s">
+        <v>34</v>
+      </c>
       <c r="L10" t="s">
         <v>34</v>
       </c>
-      <c r="M10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>32</v>
       </c>
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="M11" t="s">
+      <c r="L11" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>